<commit_message>
updated datasheets and generated mean sizes for adult families
</commit_message>
<xml_diff>
--- a/lifestage_carryover/notebooks/datasheet_example.xlsx
+++ b/lifestage_carryover/notebooks/datasheet_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/project-gigas-carryover/lifestage_carryover/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6EB8EAF-9249-F64E-AC75-6EB2DA2D2264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A27E74-2049-114E-A7AF-747F757E63B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17440" xr2:uid="{9C3F786E-3706-7444-8298-7A2F285FE399}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -50,30 +50,9 @@
     <t>tube_ID</t>
   </si>
   <si>
-    <t>conditioning_treatment</t>
-  </si>
-  <si>
-    <t>acute_treatment</t>
-  </si>
-  <si>
-    <t>number_animals</t>
-  </si>
-  <si>
-    <t>preservation_method</t>
-  </si>
-  <si>
-    <t>time_sampled</t>
-  </si>
-  <si>
-    <t>storage_location</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>replicate_tank_tag_ID</t>
-  </si>
-  <si>
     <t>orange</t>
   </si>
   <si>
@@ -86,25 +65,31 @@
     <t>stress</t>
   </si>
   <si>
-    <t>RNA/DNA shield 500uL</t>
-  </si>
-  <si>
     <t>ASH</t>
   </si>
   <si>
-    <t>Freezer A</t>
-  </si>
-  <si>
-    <t>seed</t>
-  </si>
-  <si>
-    <t>spat</t>
-  </si>
-  <si>
-    <t>spat_1</t>
-  </si>
-  <si>
-    <t>seed_1</t>
+    <t>time</t>
+  </si>
+  <si>
+    <t>conditioning treatment</t>
+  </si>
+  <si>
+    <t>acute treatment</t>
+  </si>
+  <si>
+    <t>number animals</t>
+  </si>
+  <si>
+    <t>preservation method</t>
+  </si>
+  <si>
+    <t>tag or tank</t>
+  </si>
+  <si>
+    <t>RNA later 750uL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -128,15 +113,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -144,15 +135,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,171 +482,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB08EB51-0885-5846-A825-C1479385F9B6}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L4"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="24.5" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" customWidth="1"/>
-    <col min="9" max="9" width="22.5" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="24.83203125" customWidth="1"/>
-    <col min="12" max="12" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.5" style="4" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="33.33203125" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>45350</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>45350</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="3">
         <v>0.59097222222222223</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="16" spans="1:11" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>45350</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.59375</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>45350</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.59722222222222221</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" copies="10"/>
 </worksheet>
 </file>
</xml_diff>